<commit_message>
Write data org slides
</commit_message>
<xml_diff>
--- a/slides/data/raw/tbl-01-faecal-sludge-analysis.xlsx
+++ b/slides/data/raw/tbl-01-faecal-sludge-analysis.xlsx
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>142.22</v>
+        <v>102.45</v>
       </c>
     </row>
     <row r="4">
@@ -456,7 +456,7 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n">
-        <v>98.33</v>
+        <v>57.02</v>
       </c>
     </row>
     <row r="5">
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>15.92</v>
+        <v>27.03</v>
       </c>
     </row>
     <row r="6">
@@ -707,10 +707,10 @@
         <v>45234</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E17" t="n">
         <v>26</v>
@@ -727,10 +727,10 @@
         <v>45234</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E18" t="n">
         <v>91</v>
@@ -747,10 +747,10 @@
         <v>45234</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E19" t="n">
         <v>68</v>
@@ -767,10 +767,10 @@
         <v>45234</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
         <v>112</v>
@@ -787,10 +787,10 @@
         <v>45234</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E21" t="n">
         <v>59</v>

</xml_diff>